<commit_message>
Made frustrated progress on multicog VGA driver
</commit_message>
<xml_diff>
--- a/Docs/Other/Multicog_Sandbox.xlsx
+++ b/Docs/Other/Multicog_Sandbox.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Cog 1</t>
   </si>
@@ -50,9 +50,6 @@
     <t>VERTICAL FRONT PORCH</t>
   </si>
   <si>
-    <t>This example just has 16 active video lines to keep it simple</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = porch</t>
   </si>
   <si>
@@ -62,18 +59,6 @@
     <t xml:space="preserve"> = visible video (displaying the scanline buffer)</t>
   </si>
   <si>
-    <t>10 vertical tiles</t>
-  </si>
-  <si>
-    <t>16 vertical pixels per tile</t>
-  </si>
-  <si>
-    <t>160 total pixels</t>
-  </si>
-  <si>
-    <t>3:1 scanline to tile line ratio</t>
-  </si>
-  <si>
     <t>Cog1</t>
   </si>
   <si>
@@ -86,23 +71,62 @@
     <t>↓</t>
   </si>
   <si>
-    <t>0,0</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>linesPerCog</t>
-  </si>
-  <si>
     <t>tlslRatio</t>
+  </si>
+  <si>
+    <t>sResV</t>
+  </si>
+  <si>
+    <t>vTilesV</t>
+  </si>
+  <si>
+    <t>lPerCog</t>
+  </si>
+  <si>
+    <t>startIndex</t>
+  </si>
+  <si>
+    <t>lPerTile</t>
+  </si>
+  <si>
+    <t>tSizeV</t>
+  </si>
+  <si>
+    <t>tMapIndex</t>
+  </si>
+  <si>
+    <t>(1,1)</t>
+  </si>
+  <si>
+    <t>(0,0)</t>
+  </si>
+  <si>
+    <t>slr</t>
+  </si>
+  <si>
+    <t>line#</t>
+  </si>
+  <si>
+    <t>cls</t>
+  </si>
+  <si>
+    <t>startLine</t>
+  </si>
+  <si>
+    <t>Passing into cog:</t>
+  </si>
+  <si>
+    <t>1. Initial tile palette row</t>
+  </si>
+  <si>
+    <t>2. Initial current scan line</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +162,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +227,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -219,15 +276,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -277,11 +325,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -290,12 +457,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -303,11 +464,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,6 +489,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,559 +808,718 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="29">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="26"/>
       <c r="F4" s="4"/>
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="33">
+        <v>4</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="26"/>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="10">
+        <f>(N1/N2)/N3</f>
+        <v>2</v>
+      </c>
+      <c r="V5" s="26"/>
+      <c r="X5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="26"/>
       <c r="F6" s="3"/>
       <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="12">
+        <f>FLOOR(N4/N5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="R6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="R6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="26"/>
+      <c r="X6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="7"/>
-      <c r="T7" s="24" t="s">
+      <c r="D7" s="26"/>
+      <c r="M7" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N7" s="12">
+        <f>MOD(N4,N5)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="26"/>
+      <c r="X7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="26"/>
+      <c r="M8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="14">
+        <f>N5*N3</f>
+        <v>32</v>
+      </c>
+      <c r="P8" s="38"/>
       <c r="S8" s="2"/>
-      <c r="T8" s="23">
+      <c r="T8" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U8" s="35"/>
+      <c r="V8" s="26"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="7"/>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D9" s="26"/>
+      <c r="P9" s="38"/>
       <c r="S9" s="2"/>
-      <c r="T9" s="23">
+      <c r="T9" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U9" s="35"/>
+      <c r="V9" s="26"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="7"/>
-      <c r="J10" t="s">
+      <c r="D10" s="26"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="23" t="s">
-        <v>21</v>
-      </c>
       <c r="S10" s="2"/>
-      <c r="T10" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T10" s="18">
+        <v>1</v>
+      </c>
+      <c r="U10" s="35"/>
+      <c r="V10" s="26"/>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="25" t="s">
         <v>5</v>
       </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <f>3-1</f>
+        <v>2</v>
+      </c>
       <c r="N11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="25">
+        <v>13</v>
+      </c>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" s="6"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="20">
         <v>1</v>
       </c>
-      <c r="W11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="13"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U11" s="35"/>
+      <c r="V11" s="26"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="J12">
-        <f>480/30</f>
-        <v>16</v>
-      </c>
-      <c r="N12" s="21">
+      <c r="D12" s="25"/>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="16">
         <v>0</v>
       </c>
-      <c r="Q12" s="23">
-        <v>1</v>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="18">
+        <v>2</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="29">
+      <c r="T12" s="24"/>
+      <c r="U12" s="34">
         <v>0</v>
       </c>
-      <c r="W12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="16"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V12" s="40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
-      <c r="N13" s="21">
+      <c r="D13" s="25"/>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>0</v>
       </c>
-      <c r="Q13" s="23">
-        <v>1</v>
+      <c r="N13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="18">
+        <v>2</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="29">
-        <v>0</v>
-      </c>
-      <c r="W13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T13" s="24"/>
+      <c r="U13" s="34">
+        <v>1</v>
+      </c>
+      <c r="V13" s="41"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="6"/>
-      <c r="N14" s="21">
+      <c r="D14" s="25"/>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="16">
         <v>0</v>
       </c>
-      <c r="Q14" s="23">
+      <c r="P14" s="39"/>
+      <c r="Q14" s="18">
         <v>2</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="29">
-        <v>0</v>
-      </c>
-      <c r="W14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="19"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T14" s="24"/>
+      <c r="U14" s="34">
+        <v>2</v>
+      </c>
+      <c r="V14" s="41"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="6"/>
-      <c r="N15" s="21">
+      <c r="D15" s="25"/>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="N15" s="16">
         <v>0</v>
       </c>
-      <c r="Q15" s="23">
+      <c r="P15" s="39"/>
+      <c r="Q15" s="18">
         <v>2</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T15" s="24"/>
+      <c r="U15" s="34">
+        <v>3</v>
+      </c>
+      <c r="V15" s="41"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="6"/>
-      <c r="N16" s="22">
+      <c r="D16" s="25"/>
+      <c r="N16" s="17">
         <v>0</v>
       </c>
-      <c r="Q16" s="27">
-        <v>1</v>
-      </c>
+      <c r="P16" s="38">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="22"/>
       <c r="R16" s="3"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T16" s="18">
+        <v>2</v>
+      </c>
+      <c r="U16" s="35"/>
+      <c r="V16" s="41"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="6"/>
-      <c r="N17" s="22">
+      <c r="D17" s="25"/>
+      <c r="N17" s="17">
         <v>0</v>
       </c>
-      <c r="Q17" s="27">
-        <v>1</v>
-      </c>
+      <c r="P17" s="38">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="22"/>
       <c r="R17" s="3"/>
       <c r="S17" s="2"/>
-      <c r="T17" s="23">
+      <c r="T17" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="35"/>
+      <c r="V17" s="41"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="6"/>
-      <c r="N18" s="22">
+      <c r="D18" s="25"/>
+      <c r="N18" s="17">
         <v>1</v>
       </c>
-      <c r="Q18" s="27">
-        <v>2</v>
-      </c>
+      <c r="P18" s="38">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="22"/>
       <c r="R18" s="3"/>
       <c r="S18" s="2"/>
-      <c r="T18" s="23">
+      <c r="T18" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="35"/>
+      <c r="V18" s="41"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="6"/>
-      <c r="N19" s="22">
+      <c r="D19" s="25"/>
+      <c r="N19" s="17">
         <v>1</v>
       </c>
-      <c r="Q19" s="27">
-        <v>2</v>
-      </c>
+      <c r="P19" s="38">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="22"/>
       <c r="R19" s="3"/>
       <c r="S19" s="2"/>
-      <c r="T19" s="23">
+      <c r="T19" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="35"/>
+      <c r="V19" s="41"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>10</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
-      <c r="N20" s="21">
+      <c r="D20" s="25"/>
+      <c r="N20" s="16">
         <v>1</v>
       </c>
-      <c r="Q20" s="23">
+      <c r="P20" s="39"/>
+      <c r="Q20" s="18">
         <v>4</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T20" s="22"/>
+      <c r="U20" s="34">
+        <v>8</v>
+      </c>
+      <c r="V20" s="41"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>11</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="6"/>
-      <c r="N21" s="21">
+      <c r="D21" s="25"/>
+      <c r="N21" s="16">
         <v>1</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="P21" s="39"/>
+      <c r="Q21" s="18">
         <v>4</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="3"/>
-      <c r="T21" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T21" s="22"/>
+      <c r="U21" s="34">
+        <v>9</v>
+      </c>
+      <c r="V21" s="41"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>12</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="6"/>
-      <c r="N22" s="21">
+      <c r="D22" s="25"/>
+      <c r="N22" s="16">
         <v>1</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="P22" s="39"/>
+      <c r="Q22" s="18">
         <v>4</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="3"/>
-      <c r="T22" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T22" s="22"/>
+      <c r="U22" s="34">
+        <v>10</v>
+      </c>
+      <c r="V22" s="41"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="6"/>
-      <c r="N23" s="21">
+      <c r="D23" s="25"/>
+      <c r="N23" s="16">
         <v>1</v>
       </c>
-      <c r="Q23" s="23">
+      <c r="P23" s="39"/>
+      <c r="Q23" s="18">
         <v>5</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T23" s="22"/>
+      <c r="U23" s="34">
+        <v>11</v>
+      </c>
+      <c r="V23" s="41"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>14</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
-      <c r="N24" s="22">
-        <v>2</v>
-      </c>
-      <c r="Q24" s="27">
-        <v>4</v>
-      </c>
+      <c r="D24" s="25"/>
+      <c r="N24" s="17">
+        <v>2</v>
+      </c>
+      <c r="P24" s="38">
+        <v>12</v>
+      </c>
+      <c r="Q24" s="22"/>
       <c r="R24" s="3"/>
-      <c r="T24" s="23"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24" s="34"/>
+      <c r="V24" s="41"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>15</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="6"/>
-      <c r="N25" s="22">
-        <v>2</v>
-      </c>
-      <c r="Q25" s="27">
-        <v>4</v>
-      </c>
+      <c r="D25" s="25"/>
+      <c r="N25" s="17">
+        <v>2</v>
+      </c>
+      <c r="P25" s="38">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="22"/>
       <c r="R25" s="3"/>
-      <c r="T25" s="23"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>5</v>
+      </c>
+      <c r="U25" s="34"/>
+      <c r="V25" s="41"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>16</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="6"/>
-      <c r="N26" s="22">
-        <v>2</v>
-      </c>
-      <c r="Q26" s="27">
-        <v>4</v>
-      </c>
+      <c r="D26" s="25"/>
+      <c r="N26" s="17">
+        <v>2</v>
+      </c>
+      <c r="P26" s="38">
+        <v>14</v>
+      </c>
+      <c r="Q26" s="22"/>
       <c r="R26" s="3"/>
-      <c r="T26" s="23"/>
-    </row>
-    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T26">
+        <v>6</v>
+      </c>
+      <c r="U26" s="34"/>
+      <c r="V26" s="41"/>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="N27" s="22">
-        <v>2</v>
-      </c>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="28">
-        <v>5</v>
-      </c>
-      <c r="R27" s="10"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="25"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N27" s="17">
+        <v>2</v>
+      </c>
+      <c r="P27" s="38">
+        <v>15</v>
+      </c>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6">
+        <v>6</v>
+      </c>
+      <c r="U27" s="34"/>
+      <c r="V27" s="42"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="7"/>
-      <c r="Q28" s="23"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D28" s="26"/>
+      <c r="Q28" s="18"/>
+      <c r="V28" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="7"/>
-      <c r="Q29" s="23"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D29" s="26"/>
+      <c r="Q29" s="18"/>
+      <c r="V29" s="26"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="7"/>
-      <c r="Q30" s="23"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D30" s="26"/>
+      <c r="Q30" s="18"/>
+      <c r="V30" s="26"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="7"/>
-      <c r="Q31" s="23"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D31" s="26"/>
+      <c r="Q31" s="18"/>
+      <c r="V31" s="26"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="26"/>
+      <c r="V32" s="26"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="26"/>
+      <c r="V33" s="26"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="26"/>
+      <c r="V34" s="26"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V35" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="D11:D26"/>
     <mergeCell ref="D3:D10"/>
     <mergeCell ref="D27:D34"/>
+    <mergeCell ref="V12:V27"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="V28:V35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed working initial version of multicog VGA driver
</commit_message>
<xml_diff>
--- a/Docs/Other/Multicog_Sandbox.xlsx
+++ b/Docs/Other/Multicog_Sandbox.xlsx
@@ -490,12 +490,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -518,6 +512,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -811,7 +811,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,10 +834,10 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="29">
+      <c r="N1" s="27">
         <v>480</v>
       </c>
     </row>
@@ -845,11 +845,11 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="31">
-        <v>15</v>
+      <c r="N2" s="29">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -858,13 +858,13 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="30" t="s">
+      <c r="M3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="29">
         <v>16</v>
       </c>
     </row>
@@ -874,18 +874,18 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="26"/>
+      <c r="D4" s="39"/>
       <c r="F4" s="4"/>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="31">
         <v>4</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="V4" s="39" t="s">
         <v>6</v>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="26"/>
+      <c r="D5" s="39"/>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
         <v>9</v>
@@ -905,9 +905,9 @@
       </c>
       <c r="N5" s="10">
         <f>(N1/N2)/N3</f>
-        <v>2</v>
-      </c>
-      <c r="V5" s="26"/>
+        <v>3</v>
+      </c>
+      <c r="V5" s="39"/>
       <c r="X5" t="s">
         <v>29</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="26"/>
+      <c r="D6" s="39"/>
       <c r="F6" s="3"/>
       <c r="G6" t="s">
         <v>10</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="N6" s="12">
         <f>FLOOR(N4/N5,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" s="21"/>
       <c r="R6" s="15" t="s">
@@ -940,7 +940,7 @@
       <c r="T6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="26"/>
+      <c r="V6" s="39"/>
       <c r="X6" t="s">
         <v>30</v>
       </c>
@@ -951,24 +951,24 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="26"/>
+      <c r="D7" s="39"/>
       <c r="M7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="N7" s="12">
         <f>MOD(N4,N5)</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="34" t="s">
         <v>22</v>
       </c>
       <c r="T7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="U7" s="37" t="s">
+      <c r="U7" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="V7" s="26"/>
+      <c r="V7" s="39"/>
       <c r="X7" t="s">
         <v>31</v>
       </c>
@@ -979,21 +979,21 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="26"/>
+      <c r="D8" s="39"/>
       <c r="M8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="N8" s="14">
         <f>N5*N3</f>
-        <v>32</v>
-      </c>
-      <c r="P8" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="P8" s="36"/>
       <c r="S8" s="2"/>
       <c r="T8" s="18">
         <v>0</v>
       </c>
-      <c r="U8" s="35"/>
-      <c r="V8" s="26"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="39"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1001,14 +1001,14 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="26"/>
-      <c r="P9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="P9" s="36"/>
       <c r="S9" s="2"/>
       <c r="T9" s="18">
         <v>0</v>
       </c>
-      <c r="U9" s="35"/>
-      <c r="V9" s="26"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="39"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1016,8 +1016,8 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="26"/>
-      <c r="P10" s="38"/>
+      <c r="D10" s="39"/>
+      <c r="P10" s="36"/>
       <c r="Q10" s="18" t="s">
         <v>23</v>
       </c>
@@ -1025,8 +1025,8 @@
       <c r="T10" s="18">
         <v>1</v>
       </c>
-      <c r="U10" s="35"/>
-      <c r="V10" s="26"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="39"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="38" t="s">
         <v>5</v>
       </c>
       <c r="G11" t="s">
@@ -1047,7 +1047,7 @@
       <c r="N11" t="s">
         <v>13</v>
       </c>
-      <c r="P11" s="38"/>
+      <c r="P11" s="36"/>
       <c r="Q11" s="20" t="s">
         <v>14</v>
       </c>
@@ -1056,8 +1056,8 @@
       <c r="T11" s="20">
         <v>1</v>
       </c>
-      <c r="U11" s="35"/>
-      <c r="V11" s="26"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="39"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="25"/>
+      <c r="D12" s="38"/>
       <c r="G12" t="s">
         <v>26</v>
       </c>
@@ -1075,14 +1075,14 @@
       <c r="N12" s="16">
         <v>0</v>
       </c>
-      <c r="P12" s="39"/>
+      <c r="P12" s="37"/>
       <c r="Q12" s="18">
         <v>2</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="24"/>
-      <c r="U12" s="34">
+      <c r="U12" s="32">
         <v>0</v>
       </c>
       <c r="V12" s="40" t="s">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="25"/>
+      <c r="D13" s="38"/>
       <c r="G13">
         <v>1</v>
       </c>
@@ -1105,14 +1105,14 @@
       <c r="N13" s="16">
         <v>0</v>
       </c>
-      <c r="P13" s="39"/>
+      <c r="P13" s="37"/>
       <c r="Q13" s="18">
         <v>2</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="24"/>
-      <c r="U13" s="34">
+      <c r="U13" s="32">
         <v>1</v>
       </c>
       <c r="V13" s="41"/>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="25"/>
+      <c r="D14" s="38"/>
       <c r="G14">
         <v>2</v>
       </c>
@@ -1133,14 +1133,14 @@
       <c r="N14" s="16">
         <v>0</v>
       </c>
-      <c r="P14" s="39"/>
+      <c r="P14" s="37"/>
       <c r="Q14" s="18">
         <v>2</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="24"/>
-      <c r="U14" s="34">
+      <c r="U14" s="32">
         <v>2</v>
       </c>
       <c r="V14" s="41"/>
@@ -1151,25 +1151,25 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="38"/>
       <c r="G15">
         <v>3</v>
       </c>
       <c r="H15">
         <v>2</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="25"/>
       <c r="N15" s="16">
         <v>0</v>
       </c>
-      <c r="P15" s="39"/>
+      <c r="P15" s="37"/>
       <c r="Q15" s="18">
         <v>2</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="34">
+      <c r="U15" s="32">
         <v>3</v>
       </c>
       <c r="V15" s="41"/>
@@ -1180,11 +1180,11 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="25"/>
+      <c r="D16" s="38"/>
       <c r="N16" s="17">
         <v>0</v>
       </c>
-      <c r="P16" s="38">
+      <c r="P16" s="36">
         <v>4</v>
       </c>
       <c r="Q16" s="22"/>
@@ -1193,7 +1193,7 @@
       <c r="T16" s="18">
         <v>2</v>
       </c>
-      <c r="U16" s="35"/>
+      <c r="U16" s="33"/>
       <c r="V16" s="41"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1202,11 +1202,11 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="38"/>
       <c r="N17" s="17">
         <v>0</v>
       </c>
-      <c r="P17" s="38">
+      <c r="P17" s="36">
         <v>5</v>
       </c>
       <c r="Q17" s="22"/>
@@ -1215,7 +1215,7 @@
       <c r="T17" s="18">
         <v>3</v>
       </c>
-      <c r="U17" s="35"/>
+      <c r="U17" s="33"/>
       <c r="V17" s="41"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -1224,11 +1224,11 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="38"/>
       <c r="N18" s="17">
         <v>1</v>
       </c>
-      <c r="P18" s="38">
+      <c r="P18" s="36">
         <v>6</v>
       </c>
       <c r="Q18" s="22"/>
@@ -1237,7 +1237,7 @@
       <c r="T18" s="18">
         <v>3</v>
       </c>
-      <c r="U18" s="35"/>
+      <c r="U18" s="33"/>
       <c r="V18" s="41"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -1246,11 +1246,11 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
+      <c r="D19" s="38"/>
       <c r="N19" s="17">
         <v>1</v>
       </c>
-      <c r="P19" s="38">
+      <c r="P19" s="36">
         <v>7</v>
       </c>
       <c r="Q19" s="22"/>
@@ -1259,7 +1259,7 @@
       <c r="T19" s="18">
         <v>3</v>
       </c>
-      <c r="U19" s="35"/>
+      <c r="U19" s="33"/>
       <c r="V19" s="41"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -1268,18 +1268,18 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="38"/>
       <c r="N20" s="16">
         <v>1</v>
       </c>
-      <c r="P20" s="39"/>
+      <c r="P20" s="37"/>
       <c r="Q20" s="18">
         <v>4</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="3"/>
       <c r="T20" s="22"/>
-      <c r="U20" s="34">
+      <c r="U20" s="32">
         <v>8</v>
       </c>
       <c r="V20" s="41"/>
@@ -1290,18 +1290,18 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
+      <c r="D21" s="38"/>
       <c r="N21" s="16">
         <v>1</v>
       </c>
-      <c r="P21" s="39"/>
+      <c r="P21" s="37"/>
       <c r="Q21" s="18">
         <v>4</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="3"/>
       <c r="T21" s="22"/>
-      <c r="U21" s="34">
+      <c r="U21" s="32">
         <v>9</v>
       </c>
       <c r="V21" s="41"/>
@@ -1312,18 +1312,18 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
+      <c r="D22" s="38"/>
       <c r="N22" s="16">
         <v>1</v>
       </c>
-      <c r="P22" s="39"/>
+      <c r="P22" s="37"/>
       <c r="Q22" s="18">
         <v>4</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="3"/>
       <c r="T22" s="22"/>
-      <c r="U22" s="34">
+      <c r="U22" s="32">
         <v>10</v>
       </c>
       <c r="V22" s="41"/>
@@ -1334,18 +1334,18 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="25"/>
+      <c r="D23" s="38"/>
       <c r="N23" s="16">
         <v>1</v>
       </c>
-      <c r="P23" s="39"/>
+      <c r="P23" s="37"/>
       <c r="Q23" s="18">
         <v>5</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="3"/>
       <c r="T23" s="22"/>
-      <c r="U23" s="34">
+      <c r="U23" s="32">
         <v>11</v>
       </c>
       <c r="V23" s="41"/>
@@ -1356,11 +1356,11 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="38"/>
       <c r="N24" s="17">
         <v>2</v>
       </c>
-      <c r="P24" s="38">
+      <c r="P24" s="36">
         <v>12</v>
       </c>
       <c r="Q24" s="22"/>
@@ -1368,7 +1368,7 @@
       <c r="T24">
         <v>5</v>
       </c>
-      <c r="U24" s="34"/>
+      <c r="U24" s="32"/>
       <c r="V24" s="41"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -1377,11 +1377,11 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="25"/>
+      <c r="D25" s="38"/>
       <c r="N25" s="17">
         <v>2</v>
       </c>
-      <c r="P25" s="38">
+      <c r="P25" s="36">
         <v>13</v>
       </c>
       <c r="Q25" s="22"/>
@@ -1389,7 +1389,7 @@
       <c r="T25">
         <v>5</v>
       </c>
-      <c r="U25" s="34"/>
+      <c r="U25" s="32"/>
       <c r="V25" s="41"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -1398,11 +1398,11 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="25"/>
+      <c r="D26" s="38"/>
       <c r="N26" s="17">
         <v>2</v>
       </c>
-      <c r="P26" s="38">
+      <c r="P26" s="36">
         <v>14</v>
       </c>
       <c r="Q26" s="22"/>
@@ -1410,7 +1410,7 @@
       <c r="T26">
         <v>6</v>
       </c>
-      <c r="U26" s="34"/>
+      <c r="U26" s="32"/>
       <c r="V26" s="41"/>
     </row>
     <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1419,13 +1419,13 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="39" t="s">
         <v>7</v>
       </c>
       <c r="N27" s="17">
         <v>2</v>
       </c>
-      <c r="P27" s="38">
+      <c r="P27" s="36">
         <v>15</v>
       </c>
       <c r="Q27" s="23"/>
@@ -1434,7 +1434,7 @@
       <c r="T27" s="6">
         <v>6</v>
       </c>
-      <c r="U27" s="34"/>
+      <c r="U27" s="32"/>
       <c r="V27" s="42"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -1443,9 +1443,9 @@
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="26"/>
+      <c r="D28" s="39"/>
       <c r="Q28" s="18"/>
-      <c r="V28" s="26" t="s">
+      <c r="V28" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1455,9 +1455,9 @@
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="26"/>
+      <c r="D29" s="39"/>
       <c r="Q29" s="18"/>
-      <c r="V29" s="26"/>
+      <c r="V29" s="39"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1465,9 +1465,9 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="26"/>
+      <c r="D30" s="39"/>
       <c r="Q30" s="18"/>
-      <c r="V30" s="26"/>
+      <c r="V30" s="39"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1475,9 +1475,9 @@
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="26"/>
+      <c r="D31" s="39"/>
       <c r="Q31" s="18"/>
-      <c r="V31" s="26"/>
+      <c r="V31" s="39"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1485,8 +1485,8 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="26"/>
-      <c r="V32" s="26"/>
+      <c r="D32" s="39"/>
+      <c r="V32" s="39"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1494,8 +1494,8 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="26"/>
-      <c r="V33" s="26"/>
+      <c r="D33" s="39"/>
+      <c r="V33" s="39"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1503,14 +1503,14 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="26"/>
-      <c r="V34" s="26"/>
+      <c r="D34" s="39"/>
+      <c r="V34" s="39"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V35" s="26"/>
+      <c r="V35" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>